<commit_message>
HP: Student feedback info adding and safe command coding
</commit_message>
<xml_diff>
--- a/xmlChecker/data/project_U1_sub1/students_U1_2.xlsx
+++ b/xmlChecker/data/project_U1_sub1/students_U1_2.xlsx
@@ -370,6 +370,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -834,9 +835,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="45.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="45.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1168,7 +1169,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="29.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" customWidth="true" width="29.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1303,9 +1304,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -1454,22 +1455,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="37.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="29.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="29.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="37.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="29.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">

</xml_diff>